<commit_message>
Changes to design doc
</commit_message>
<xml_diff>
--- a/Design doc.xlsx
+++ b/Design doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Stock market investment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1542A37-8090-437A-82F3-5F9FD78DD14E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C00301-D5A2-495A-878D-7B4F74450377}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8BD4D62F-CA13-407D-B30F-E9A78808E7C9}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Quarterly" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Yearly!$A$5:$BO$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Yearly!$A$5:$BU$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
   <si>
     <t>Company Name</t>
   </si>
@@ -52,15 +52,6 @@
     <t>Net Profit</t>
   </si>
   <si>
-    <t>Net Profit % of increase/Decrease</t>
-  </si>
-  <si>
-    <t>Revenue % of Increase/Decrease</t>
-  </si>
-  <si>
-    <t>Profit % of Increase/Decrease</t>
-  </si>
-  <si>
     <t>Sales = Revenue</t>
   </si>
   <si>
@@ -76,27 +67,6 @@
     <t>Trent</t>
   </si>
   <si>
-    <t>For now start with below companies</t>
-  </si>
-  <si>
-    <t>Reliance</t>
-  </si>
-  <si>
-    <t>2008-2019</t>
-  </si>
-  <si>
-    <t>2009-2020</t>
-  </si>
-  <si>
-    <t>SBI cards</t>
-  </si>
-  <si>
-    <t>2014-2019</t>
-  </si>
-  <si>
-    <t>Years</t>
-  </si>
-  <si>
     <t>Idea</t>
   </si>
   <si>
@@ -133,9 +103,6 @@
     <t>EPS</t>
   </si>
   <si>
-    <t>Book value/Share</t>
-  </si>
-  <si>
     <t>Interest Coverage Ratios</t>
   </si>
   <si>
@@ -176,6 +143,93 @@
   </si>
   <si>
     <t>avg ROE for past 5 yrs should be &gt;=20%</t>
+  </si>
+  <si>
+    <t>Valuation</t>
+  </si>
+  <si>
+    <t>P/E</t>
+  </si>
+  <si>
+    <t>Compare with its historical average and if its trading less than its historical avg P/E could be a buy</t>
+  </si>
+  <si>
+    <t>Compare with its peers</t>
+  </si>
+  <si>
+    <t>Compare with sensex</t>
+  </si>
+  <si>
+    <t>higher growth higher PE</t>
+  </si>
+  <si>
+    <t>Massive cashflow and less leveraged</t>
+  </si>
+  <si>
+    <t>Lower the P/B the better</t>
+  </si>
+  <si>
+    <t>Current PE is not more than two times of the last three years average earnings growth rate</t>
+  </si>
+  <si>
+    <t>PEG = PE/Earning growth rate</t>
+  </si>
+  <si>
+    <t>PEG&lt;0.5</t>
+  </si>
+  <si>
+    <t>undervalued and could be an opportunity</t>
+  </si>
+  <si>
+    <t>0.5&lt;PEG&lt;1</t>
+  </si>
+  <si>
+    <t>undervalued or resonably valued</t>
+  </si>
+  <si>
+    <t>1&lt;PEG&lt;2</t>
+  </si>
+  <si>
+    <t>Reasonably valued</t>
+  </si>
+  <si>
+    <t>PEG&gt;2</t>
+  </si>
+  <si>
+    <t>Over valued</t>
+  </si>
+  <si>
+    <t>PEG is calculated for past 3yrs</t>
+  </si>
+  <si>
+    <t>Calculated for past 5 yrs</t>
+  </si>
+  <si>
+    <t>Undervalued</t>
+  </si>
+  <si>
+    <t>Fairly valued</t>
+  </si>
+  <si>
+    <t>PEG</t>
+  </si>
+  <si>
+    <t>Avg PE (5 yrs)</t>
+  </si>
+  <si>
+    <t>EPS CAGR(3 yrs)</t>
+  </si>
+  <si>
+    <t>Valuation based on P/E and PEG ratio</t>
+  </si>
+  <si>
+    <t>Current P/E</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Sector/Industry</t>
   </si>
 </sst>
 </file>
@@ -299,9 +353,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -309,6 +360,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,106 +679,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4B59EE-406E-4588-820C-A407EF25A70E}">
-  <dimension ref="A1:BP31"/>
+  <dimension ref="A1:BV52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="6" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.109375" customWidth="1"/>
-    <col min="37" max="37" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" customWidth="1"/>
+    <col min="13" max="13" width="6" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="14.33203125" customWidth="1"/>
+    <col min="23" max="23" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="W2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -738,312 +799,330 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="9">
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="8">
         <v>2020</v>
       </c>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="9">
-        <f>Q4-1</f>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="8">
+        <f>W4-1</f>
         <v>2019</v>
       </c>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="9">
-        <f>U4-1</f>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="8">
+        <f>AA4-1</f>
         <v>2018</v>
       </c>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="9">
-        <f>Y4-1</f>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="10"/>
+      <c r="AI4" s="8">
+        <f>AE4-1</f>
         <v>2017</v>
       </c>
-      <c r="AD4" s="10"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="11"/>
-      <c r="AG4" s="9">
-        <f>AC4-1</f>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="9"/>
+      <c r="AL4" s="10"/>
+      <c r="AM4" s="8">
+        <f>AI4-1</f>
         <v>2016</v>
       </c>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="11"/>
-      <c r="AK4" s="9">
-        <f t="shared" ref="AK4" si="0">AG4-1</f>
+      <c r="AN4" s="9"/>
+      <c r="AO4" s="9"/>
+      <c r="AP4" s="10"/>
+      <c r="AQ4" s="8">
+        <f t="shared" ref="AQ4" si="0">AM4-1</f>
         <v>2015</v>
       </c>
-      <c r="AL4" s="10"/>
-      <c r="AM4" s="10"/>
-      <c r="AN4" s="11"/>
-      <c r="AO4" s="9">
-        <f t="shared" ref="AO4" si="1">AK4-1</f>
+      <c r="AR4" s="9"/>
+      <c r="AS4" s="9"/>
+      <c r="AT4" s="10"/>
+      <c r="AU4" s="8">
+        <f t="shared" ref="AU4" si="1">AQ4-1</f>
         <v>2014</v>
       </c>
-      <c r="AP4" s="10"/>
-      <c r="AQ4" s="10"/>
-      <c r="AR4" s="11"/>
-      <c r="AS4" s="9">
-        <f t="shared" ref="AS4" si="2">AO4-1</f>
+      <c r="AV4" s="9"/>
+      <c r="AW4" s="9"/>
+      <c r="AX4" s="10"/>
+      <c r="AY4" s="8">
+        <f t="shared" ref="AY4" si="2">AU4-1</f>
         <v>2013</v>
       </c>
-      <c r="AT4" s="10"/>
-      <c r="AU4" s="10"/>
-      <c r="AV4" s="11"/>
-      <c r="AW4" s="9">
-        <f t="shared" ref="AW4" si="3">AS4-1</f>
+      <c r="AZ4" s="9"/>
+      <c r="BA4" s="9"/>
+      <c r="BB4" s="10"/>
+      <c r="BC4" s="8">
+        <f t="shared" ref="BC4" si="3">AY4-1</f>
         <v>2012</v>
       </c>
-      <c r="AX4" s="10"/>
-      <c r="AY4" s="10"/>
-      <c r="AZ4" s="11"/>
-      <c r="BA4" s="9">
-        <f t="shared" ref="BA4" si="4">AW4-1</f>
+      <c r="BD4" s="9"/>
+      <c r="BE4" s="9"/>
+      <c r="BF4" s="10"/>
+      <c r="BG4" s="8">
+        <f t="shared" ref="BG4" si="4">BC4-1</f>
         <v>2011</v>
       </c>
-      <c r="BB4" s="10"/>
-      <c r="BC4" s="10"/>
-      <c r="BD4" s="11"/>
-      <c r="BE4" s="9">
-        <f t="shared" ref="BE4" si="5">BA4-1</f>
+      <c r="BH4" s="9"/>
+      <c r="BI4" s="9"/>
+      <c r="BJ4" s="10"/>
+      <c r="BK4" s="8">
+        <f t="shared" ref="BK4" si="5">BG4-1</f>
         <v>2010</v>
       </c>
-      <c r="BF4" s="10"/>
-      <c r="BG4" s="10"/>
-      <c r="BH4" s="11"/>
-      <c r="BI4" s="9">
-        <f t="shared" ref="BI4" si="6">BE4-1</f>
+      <c r="BL4" s="9"/>
+      <c r="BM4" s="9"/>
+      <c r="BN4" s="10"/>
+      <c r="BO4" s="8">
+        <f t="shared" ref="BO4" si="6">BK4-1</f>
         <v>2009</v>
       </c>
-      <c r="BJ4" s="10"/>
-      <c r="BK4" s="10"/>
-      <c r="BL4" s="11"/>
-      <c r="BM4" s="8">
-        <f t="shared" ref="BM4" si="7">BI4-1</f>
+      <c r="BP4" s="9"/>
+      <c r="BQ4" s="9"/>
+      <c r="BR4" s="10"/>
+      <c r="BS4" s="11">
+        <f t="shared" ref="BS4" si="7">BO4-1</f>
         <v>2008</v>
       </c>
-      <c r="BN4" s="8"/>
-      <c r="BO4" s="8"/>
-      <c r="BP4" s="8"/>
-    </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="BT4" s="11"/>
+      <c r="BU4" s="11"/>
+      <c r="BV4" s="11"/>
+    </row>
+    <row r="5" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="N5" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="Q5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="X5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="Y5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="T5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="U5" s="3" t="s">
+      <c r="Z5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="V5" s="3" t="s">
+      <c r="AB5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="W5" s="3" t="s">
+      <c r="AC5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="X5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y5" s="3" t="s">
+      <c r="AD5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Z5" s="3" t="s">
+      <c r="AF5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AA5" s="3" t="s">
+      <c r="AG5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AB5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC5" s="3" t="s">
+      <c r="AH5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AD5" s="3" t="s">
+      <c r="AJ5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AE5" s="3" t="s">
+      <c r="AK5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AF5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG5" s="3" t="s">
+      <c r="AL5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AH5" s="3" t="s">
+      <c r="AN5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AI5" s="3" t="s">
+      <c r="AO5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AJ5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK5" s="3" t="s">
+      <c r="AP5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AQ5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AL5" s="3" t="s">
+      <c r="AR5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AM5" s="3" t="s">
+      <c r="AS5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AN5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AO5" s="3" t="s">
+      <c r="AT5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AU5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AP5" s="3" t="s">
+      <c r="AV5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AQ5" s="3" t="s">
+      <c r="AW5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AR5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AS5" s="3" t="s">
+      <c r="AX5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AY5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AT5" s="3" t="s">
+      <c r="AZ5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AU5" s="3" t="s">
+      <c r="BA5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AV5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AW5" s="3" t="s">
+      <c r="BB5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="BC5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AX5" s="3" t="s">
+      <c r="BD5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AY5" s="3" t="s">
+      <c r="BE5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AZ5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="BA5" s="3" t="s">
+      <c r="BF5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="BG5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="BB5" s="3" t="s">
+      <c r="BH5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="BC5" s="3" t="s">
+      <c r="BI5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="BD5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="BE5" s="3" t="s">
+      <c r="BJ5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="BK5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="BF5" s="3" t="s">
+      <c r="BL5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="BG5" s="3" t="s">
+      <c r="BM5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="BH5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="BI5" s="3" t="s">
+      <c r="BN5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="BO5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="BJ5" s="3" t="s">
+      <c r="BP5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="BK5" s="3" t="s">
+      <c r="BQ5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="BL5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="BM5" s="7" t="s">
+      <c r="BR5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="BS5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="BN5" s="3" t="s">
+      <c r="BT5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="BO5" s="3" t="s">
+      <c r="BU5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="BP5" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="BV5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="1">
         <v>687.4</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1053,149 +1132,146 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="1">
-        <f>((U6-BM6)/BM6)*100</f>
-        <v>318.978102189781</v>
-      </c>
-      <c r="O6" s="1">
-        <f>((V6-BN6)/BN6)*100</f>
-        <v>628.125</v>
-      </c>
-      <c r="P6" s="1">
-        <f>((W6-BO6)/BO6)*100</f>
-        <v>185.29411764705884</v>
-      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
-      <c r="U6" s="1">
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1">
         <v>2870</v>
       </c>
-      <c r="V6" s="1">
+      <c r="AB6" s="1">
         <v>233</v>
       </c>
-      <c r="W6" s="1">
+      <c r="AC6" s="1">
         <v>97</v>
       </c>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1">
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1">
         <v>2347</v>
       </c>
-      <c r="Z6" s="1">
+      <c r="AF6" s="1">
         <v>205</v>
       </c>
-      <c r="AA6" s="1">
+      <c r="AG6" s="1">
         <v>87</v>
       </c>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1">
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1">
         <v>1812</v>
       </c>
-      <c r="AD6" s="1">
+      <c r="AJ6" s="1">
         <v>128</v>
       </c>
-      <c r="AE6" s="1">
+      <c r="AK6" s="1">
         <v>85</v>
       </c>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1">
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1">
         <v>1686</v>
       </c>
-      <c r="AH6" s="1">
+      <c r="AN6" s="1">
         <v>100</v>
       </c>
-      <c r="AI6" s="1">
+      <c r="AO6" s="1">
         <v>55</v>
       </c>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="1">
+      <c r="AP6" s="1"/>
+      <c r="AQ6" s="1">
         <v>2284</v>
       </c>
-      <c r="AL6" s="1">
+      <c r="AR6" s="1">
         <v>41</v>
       </c>
-      <c r="AM6" s="1">
+      <c r="AS6" s="1">
         <v>129</v>
       </c>
-      <c r="AN6" s="1"/>
-      <c r="AO6" s="1">
+      <c r="AT6" s="1"/>
+      <c r="AU6" s="1">
         <v>2333</v>
       </c>
-      <c r="AP6" s="1">
+      <c r="AV6" s="1">
         <v>10</v>
       </c>
-      <c r="AQ6" s="1">
+      <c r="AW6" s="1">
         <v>-19</v>
       </c>
-      <c r="AR6" s="1"/>
-      <c r="AS6" s="1">
+      <c r="AX6" s="1"/>
+      <c r="AY6" s="1">
         <v>2132</v>
       </c>
-      <c r="AT6" s="1">
+      <c r="AZ6" s="1">
         <v>-6</v>
       </c>
-      <c r="AU6" s="1">
+      <c r="BA6" s="1">
         <v>-27</v>
       </c>
-      <c r="AV6" s="1"/>
-      <c r="AW6" s="1">
+      <c r="BB6" s="1"/>
+      <c r="BC6" s="1">
         <v>1845</v>
       </c>
-      <c r="AX6" s="1">
+      <c r="BD6" s="1">
         <v>-55</v>
       </c>
-      <c r="AY6" s="1">
+      <c r="BE6" s="1">
         <v>-38</v>
       </c>
-      <c r="AZ6" s="1"/>
-      <c r="BA6" s="1">
+      <c r="BF6" s="1"/>
+      <c r="BG6" s="1">
         <v>1511</v>
       </c>
-      <c r="BB6" s="1">
+      <c r="BH6" s="1">
         <v>22</v>
       </c>
-      <c r="BC6" s="1">
+      <c r="BI6" s="1">
         <v>7</v>
       </c>
-      <c r="BD6" s="1"/>
-      <c r="BE6" s="1">
+      <c r="BJ6" s="1"/>
+      <c r="BK6" s="1">
         <v>1052</v>
       </c>
-      <c r="BF6" s="1">
+      <c r="BL6" s="1">
         <v>5</v>
       </c>
-      <c r="BG6" s="1">
+      <c r="BM6" s="1">
         <v>2</v>
       </c>
-      <c r="BH6" s="1"/>
-      <c r="BI6" s="1">
+      <c r="BN6" s="1"/>
+      <c r="BO6" s="1">
         <v>810</v>
       </c>
-      <c r="BJ6" s="1">
+      <c r="BP6" s="1">
         <v>-4</v>
       </c>
-      <c r="BK6" s="1">
+      <c r="BQ6" s="1">
         <v>1</v>
       </c>
-      <c r="BL6" s="1"/>
-      <c r="BM6" s="1">
+      <c r="BR6" s="1"/>
+      <c r="BS6" s="1">
         <v>685</v>
       </c>
-      <c r="BN6" s="1">
+      <c r="BT6" s="1">
         <v>32</v>
       </c>
-      <c r="BO6" s="1">
+      <c r="BU6" s="1">
         <v>34</v>
       </c>
-      <c r="BP6" s="1"/>
-    </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="BV6" s="1"/>
+    </row>
+    <row r="7" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1261,116 +1337,225 @@
       <c r="BN7" s="1"/>
       <c r="BO7" s="1"/>
       <c r="BP7" s="1"/>
-    </row>
-    <row r="11" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
+      <c r="BQ7" s="1"/>
+      <c r="BR7" s="1"/>
+      <c r="BS7" s="1"/>
+      <c r="BT7" s="1"/>
+      <c r="BU7" s="1"/>
+      <c r="BV7" s="1"/>
+    </row>
+    <row r="11" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="N11" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="N12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="N13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="N14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="K46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>46</v>
+      </c>
+      <c r="D47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="K52" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="U4:X4"/>
-    <mergeCell ref="Y4:AB4"/>
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="BM4:BP4"/>
-    <mergeCell ref="AG4:AJ4"/>
-    <mergeCell ref="AK4:AN4"/>
-    <mergeCell ref="AO4:AR4"/>
-    <mergeCell ref="AS4:AV4"/>
-    <mergeCell ref="AW4:AZ4"/>
-    <mergeCell ref="BA4:BD4"/>
-    <mergeCell ref="BE4:BH4"/>
-    <mergeCell ref="BI4:BL4"/>
+    <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="AA4:AD4"/>
+    <mergeCell ref="AE4:AH4"/>
+    <mergeCell ref="AI4:AL4"/>
+    <mergeCell ref="BS4:BV4"/>
+    <mergeCell ref="AM4:AP4"/>
+    <mergeCell ref="AQ4:AT4"/>
+    <mergeCell ref="AU4:AX4"/>
+    <mergeCell ref="AY4:BB4"/>
+    <mergeCell ref="BC4:BF4"/>
+    <mergeCell ref="BG4:BJ4"/>
+    <mergeCell ref="BK4:BN4"/>
+    <mergeCell ref="BO4:BR4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1389,7 +1574,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>